<commit_message>
adding new brute force runtimes
</commit_message>
<xml_diff>
--- a/Runtimes and Plots.xlsx
+++ b/Runtimes and Plots.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7527107\source\repos\BETSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517DD5BB-B9BB-48CA-A890-B5D88D93A3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541530A1-AD23-4D16-80EF-A0B2BE012272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{332BB2C1-9D0D-4F98-990D-5C125C10D63B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="brute force" sheetId="1" r:id="rId1"/>
+    <sheet name="dynamic programming" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Input Size</t>
   </si>
@@ -44,10 +45,19 @@
     <t>Time to run</t>
   </si>
   <si>
-    <t>Factorialization</t>
+    <t>n squared</t>
   </si>
   <si>
-    <t>factorial</t>
+    <t>quadraticalization</t>
+  </si>
+  <si>
+    <t>runtime / n!</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>n!</t>
   </si>
 </sst>
 </file>
@@ -157,11 +167,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'brute force'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time to run</c:v>
+                  <c:v>Runtime</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -190,10 +200,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'brute force'!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -223,16 +233,22 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>'brute force'!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
@@ -240,28 +256,34 @@
                   <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4000000000000002E-2</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7E-2</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>2.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.02</c:v>
+                  <c:v>0.23499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.754999999999995</c:v>
+                  <c:v>1.9950000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1122.402</c:v>
+                  <c:v>21.605</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11705.569</c:v>
+                  <c:v>264.20400000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2626.1529999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37946.434999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -305,6 +327,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Input</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Size (n)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -367,6 +449,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -515,11 +657,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'brute force'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Factorialization</c:v>
+                  <c:v>runtime / n!</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -548,10 +690,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>'brute force'!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -581,16 +723,22 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:f>'brute force'!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>5.0000000000000001E-4</c:v>
                 </c:pt>
@@ -598,28 +746,34 @@
                   <c:v>1.25E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3333333333333335E-5</c:v>
+                  <c:v>2.5000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.7222222222222228E-5</c:v>
+                  <c:v>4.1666666666666669E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3253968253968251E-6</c:v>
+                  <c:v>1.388888888888889E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.388888888888889E-5</c:v>
+                  <c:v>7.1924603174603183E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9345238095238094E-5</c:v>
+                  <c:v>6.4759700176366836E-7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4734071869488534E-5</c:v>
+                  <c:v>5.4976851851851858E-7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8118536556036557E-5</c:v>
+                  <c:v>5.4125080166746837E-7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4437431941772219E-5</c:v>
+                  <c:v>5.5157227032227034E-7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.2173506149200591E-7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.3527390222578714E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -627,7 +781,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-45B2-47CB-9888-E30BE3DEEE83}"/>
+              <c16:uniqueId val="{00000000-6450-4B29-B7AB-3DA87DC403F3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -639,11 +793,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="323498176"/>
-        <c:axId val="323500256"/>
+        <c:axId val="1544479856"/>
+        <c:axId val="1544476528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="323498176"/>
+        <c:axId val="1544479856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,6 +817,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Input Size (n)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -700,12 +909,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="323500256"/>
+        <c:crossAx val="1544476528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="323500256"/>
+        <c:axId val="1544476528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,6 +934,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>runtime</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> / n!</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -762,7 +1031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="323498176"/>
+        <c:crossAx val="1544479856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1934,16 +2203,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>168910</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>77258</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>494875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>22224</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>260349</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>77258</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>258233</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1970,23 +2239,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>139701</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>55034</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>469901</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>135467</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>237068</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>67734</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>287867</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>156633</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D605DB50-1FD8-0A3A-454E-AC4984531443}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59702080-8227-AF17-01F7-8362DE73E29D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2304,26 +2573,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA9780CE-B1E2-4F24-80A3-CE8F5C5D4FC7}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="25.68359375" customWidth="1"/>
+    <col min="3" max="3" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2335,12 +2609,12 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C2">
-        <f>B2/(FACT(A2))</f>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="D2">
         <f>FACT(A2)</f>
         <v>6</v>
+      </c>
+      <c r="D2">
+        <f>B2/C2</f>
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2352,152 +2626,556 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C11" si="0">B3/(FACT(A3))</f>
+        <f>FACT(A3)</f>
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D13" si="0">B3/C3</f>
         <v>1.25E-4</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D11" si="1">FACT(A3)</f>
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <f t="shared" ref="A4:A12" si="2">A3+1</f>
+        <f t="shared" ref="A4:A11" si="1">A3+1</f>
         <v>5</v>
       </c>
       <c r="B4">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C4">
+        <f>FACT(A4)</f>
+        <v>120</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335E-5</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <v>2.5000000000000001E-5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3.4000000000000002E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C5">
+        <f>FACT(A5)</f>
+        <v>720</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
-        <v>4.7222222222222228E-5</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>720</v>
+        <v>4.1666666666666669E-6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B6">
-        <v>4.7E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="C6">
+        <f>FACT(A6)</f>
+        <v>5040</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>9.3253968253968251E-6</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>5040</v>
+        <v>1.388888888888889E-6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.56000000000000005</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="C7">
+        <f>FACT(A7)</f>
+        <v>40320</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
-        <v>1.388888888888889E-5</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>40320</v>
+        <v>7.1924603174603183E-7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B8">
-        <v>7.02</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="C8">
+        <f>FACT(A8)</f>
+        <v>362880</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>1.9345238095238094E-5</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
-        <v>362880</v>
+        <v>6.4759700176366836E-7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B9">
-        <v>89.754999999999995</v>
+        <v>1.9950000000000001</v>
       </c>
       <c r="C9">
+        <f>FACT(A9)</f>
+        <v>3628800</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>2.4734071869488534E-5</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>3628800</v>
+        <v>5.4976851851851858E-7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B10">
-        <v>1122.402</v>
+        <v>21.605</v>
       </c>
       <c r="C10">
+        <f>FACT(A10)</f>
+        <v>39916800</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
-        <v>2.8118536556036557E-5</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="1"/>
-        <v>39916800</v>
+        <v>5.4125080166746837E-7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B11">
-        <v>11705.569</v>
+        <v>264.20400000000001</v>
       </c>
       <c r="C11">
+        <f>FACT(A11)</f>
+        <v>479001600</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
-        <v>2.4437431941772219E-5</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="1"/>
-        <v>479001600</v>
+        <v>5.5157227032227034E-7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>2626.1529999999998</v>
+      </c>
+      <c r="C12">
+        <f>FACT(A12)</f>
+        <v>6227020800</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>4.2173506149200591E-7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>37946.434999999998</v>
+      </c>
+      <c r="C13">
+        <f>FACT(A13)</f>
+        <v>87178291200</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>4.3527390222578714E-7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4663E475-D24F-4087-AB4D-B10EF96395A9}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="10.3125" customWidth="1"/>
+    <col min="3" max="3" width="14.83984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>2E-3</v>
+      </c>
+      <c r="C2">
+        <f>B2/(A2*A2)</f>
+        <v>1.25E-4</v>
+      </c>
+      <c r="D2">
+        <f>A2*A2</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2E-3</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C25" si="0">B3/(A3*A3)</f>
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D25" si="1">A3*A3</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2E-3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555558E-5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2E-3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>4.0816326530612245E-5</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4.6875000000000001E-5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3.7037037037037037E-5</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2.4793388429752065E-5</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333333E-5</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>676</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>729</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>